<commit_message>
230904, 0828, 0911, 0918 modified
</commit_message>
<xml_diff>
--- a/data/quiz230911.xlsx
+++ b/data/quiz230911.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kwlee/My_Google_Drive/Works/Class/Statistics/R.WD/Class_data/class202302/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC4547BA-528E-024A-A731-76202F5A6670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B807603D-40A1-5B44-B8CA-1BF43250653F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-36640" yWindow="500" windowWidth="33200" windowHeight="19340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5233" uniqueCount="1285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5404" uniqueCount="1325">
   <si>
     <t>타임스탬프</t>
   </si>
@@ -3875,6 +3875,126 @@
   </si>
   <si>
     <t>이유빈</t>
+  </si>
+  <si>
+    <t>hshs0104746@naver.com</t>
+  </si>
+  <si>
+    <t>최희수</t>
+  </si>
+  <si>
+    <t>ehdus040127@naver.com</t>
+  </si>
+  <si>
+    <t>hjkiubb@naver.com</t>
+  </si>
+  <si>
+    <t>박재은</t>
+  </si>
+  <si>
+    <t>smile001118@naver.com</t>
+  </si>
+  <si>
+    <t>홍성준</t>
+  </si>
+  <si>
+    <t>poliku8630@naver.com</t>
+  </si>
+  <si>
+    <t>컨텐츠 IT</t>
+  </si>
+  <si>
+    <t>심지혁</t>
+  </si>
+  <si>
+    <t>hyeeun7356@gmail.com</t>
+  </si>
+  <si>
+    <t>유혜은</t>
+  </si>
+  <si>
+    <t>dnjsgmlwjd1020@naver.com</t>
+  </si>
+  <si>
+    <t>원희정</t>
+  </si>
+  <si>
+    <t>minjeong7432@gmail.com</t>
+  </si>
+  <si>
+    <t>김민정</t>
+  </si>
+  <si>
+    <t>alsgk03@naver.com</t>
+  </si>
+  <si>
+    <t>박민하</t>
+  </si>
+  <si>
+    <t>suani3176@gmail.com</t>
+  </si>
+  <si>
+    <t>박수안</t>
+  </si>
+  <si>
+    <t>hkmcosmos1@gmail.com</t>
+  </si>
+  <si>
+    <t>글로벌 비즈니스</t>
+  </si>
+  <si>
+    <t>한기민</t>
+  </si>
+  <si>
+    <t>yeon-jin22@naver.com</t>
+  </si>
+  <si>
+    <t>최연진</t>
+  </si>
+  <si>
+    <t>bsw030409@naver.com</t>
+  </si>
+  <si>
+    <t>백승우</t>
+  </si>
+  <si>
+    <t>hyj4213@naver.com</t>
+  </si>
+  <si>
+    <t>함영준</t>
+  </si>
+  <si>
+    <t>seo1020102p@naver.com</t>
+  </si>
+  <si>
+    <t>박재연</t>
+  </si>
+  <si>
+    <t>kddong99@gmail.com</t>
+  </si>
+  <si>
+    <t>빅데이터전공</t>
+  </si>
+  <si>
+    <t>김상준</t>
+  </si>
+  <si>
+    <t>psjj3840@gmail.com</t>
+  </si>
+  <si>
+    <t>박서진</t>
+  </si>
+  <si>
+    <t>ub030801@naver.com</t>
+  </si>
+  <si>
+    <t>신유빈</t>
+  </si>
+  <si>
+    <t>yenaridia@naver.com</t>
+  </si>
+  <si>
+    <t>최예나</t>
   </si>
 </sst>
 </file>
@@ -4151,11 +4271,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:N581"/>
+  <dimension ref="A1:N600"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A537" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G553" sqref="G553"/>
+      <pane ySplit="1" topLeftCell="A567" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F578" sqref="F578"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -27987,6 +28107,785 @@
         <v>22</v>
       </c>
     </row>
+    <row r="582" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A582" s="2">
+        <v>45189.947905763889</v>
+      </c>
+      <c r="B582" s="1" t="s">
+        <v>1285</v>
+      </c>
+      <c r="C582" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D582" s="1">
+        <v>20232639</v>
+      </c>
+      <c r="E582" s="1" t="s">
+        <v>1286</v>
+      </c>
+      <c r="F582" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G582" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H582" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I582" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J582" s="5">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="K582" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L582" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M582" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="583" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A583" s="2">
+        <v>45189.977292071759</v>
+      </c>
+      <c r="B583" s="1" t="s">
+        <v>1287</v>
+      </c>
+      <c r="C583" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D583" s="1">
+        <v>20232307</v>
+      </c>
+      <c r="E583" s="1" t="s">
+        <v>615</v>
+      </c>
+      <c r="F583" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G583" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H583" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I583" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J583" s="5">
+        <v>2E-3</v>
+      </c>
+      <c r="K583" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L583" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N583" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="584" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A584" s="2">
+        <v>45190.023082974541</v>
+      </c>
+      <c r="B584" s="1" t="s">
+        <v>1288</v>
+      </c>
+      <c r="C584" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D584" s="1">
+        <v>20232538</v>
+      </c>
+      <c r="E584" s="1" t="s">
+        <v>1289</v>
+      </c>
+      <c r="F584" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G584" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H584" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I584" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J584" s="5">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="K584" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L584" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N584" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="585" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A585" s="2">
+        <v>45190.032196400462</v>
+      </c>
+      <c r="B585" s="1" t="s">
+        <v>1290</v>
+      </c>
+      <c r="C585" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="D585" s="1">
+        <v>20222240</v>
+      </c>
+      <c r="E585" s="1" t="s">
+        <v>1291</v>
+      </c>
+      <c r="F585" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G585" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H585" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I585" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J585" s="5">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="K585" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L585" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M585" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="586" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A586" s="2">
+        <v>45190.072204861106</v>
+      </c>
+      <c r="B586" s="1" t="s">
+        <v>1292</v>
+      </c>
+      <c r="C586" s="1" t="s">
+        <v>1293</v>
+      </c>
+      <c r="D586" s="1">
+        <v>20205197</v>
+      </c>
+      <c r="E586" s="1" t="s">
+        <v>1294</v>
+      </c>
+      <c r="F586" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G586" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H586" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I586" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J586" s="5">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="K586" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L586" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M586" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="587" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A587" s="2">
+        <v>45190.072562233792</v>
+      </c>
+      <c r="B587" s="1" t="s">
+        <v>1295</v>
+      </c>
+      <c r="C587" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="D587" s="1">
+        <v>20203824</v>
+      </c>
+      <c r="E587" s="1" t="s">
+        <v>1296</v>
+      </c>
+      <c r="F587" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G587" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H587" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I587" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J587" s="5">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="K587" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L587" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N587" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="588" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A588" s="2">
+        <v>45190.145193090277</v>
+      </c>
+      <c r="B588" s="1" t="s">
+        <v>1297</v>
+      </c>
+      <c r="C588" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D588" s="1">
+        <v>20231057</v>
+      </c>
+      <c r="E588" s="1" t="s">
+        <v>1298</v>
+      </c>
+      <c r="F588" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G588" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H588" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I588" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J588" s="5">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="K588" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L588" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N588" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="589" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A589" s="2">
+        <v>45190.384077395836</v>
+      </c>
+      <c r="B589" s="1" t="s">
+        <v>1299</v>
+      </c>
+      <c r="C589" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D589" s="1">
+        <v>20236217</v>
+      </c>
+      <c r="E589" s="1" t="s">
+        <v>1300</v>
+      </c>
+      <c r="F589" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G589" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H589" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I589" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J589" s="5">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="K589" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L589" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N589" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="590" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A590" s="2">
+        <v>45190.41397086806</v>
+      </c>
+      <c r="B590" s="1" t="s">
+        <v>1301</v>
+      </c>
+      <c r="C590" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="D590" s="1">
+        <v>20222213</v>
+      </c>
+      <c r="E590" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F590" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G590" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H590" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I590" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J590" s="5">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="K590" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L590" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N590" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="591" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A591" s="2">
+        <v>45190.523514513887</v>
+      </c>
+      <c r="B591" s="1" t="s">
+        <v>1303</v>
+      </c>
+      <c r="C591" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D591" s="1">
+        <v>20232328</v>
+      </c>
+      <c r="E591" s="1" t="s">
+        <v>1304</v>
+      </c>
+      <c r="F591" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G591" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H591" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I591" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J591" s="5">
+        <v>0.374</v>
+      </c>
+      <c r="K591" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L591" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N591" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="592" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A592" s="2">
+        <v>45190.588201342594</v>
+      </c>
+      <c r="B592" s="1" t="s">
+        <v>1305</v>
+      </c>
+      <c r="C592" s="1" t="s">
+        <v>1306</v>
+      </c>
+      <c r="D592" s="1">
+        <v>20226429</v>
+      </c>
+      <c r="E592" s="1" t="s">
+        <v>1307</v>
+      </c>
+      <c r="F592" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G592" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="H592" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I592" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J592" s="5">
+        <v>0.151</v>
+      </c>
+      <c r="K592" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L592" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N592" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="593" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A593" s="2">
+        <v>45190.610064074077</v>
+      </c>
+      <c r="B593" s="1" t="s">
+        <v>1308</v>
+      </c>
+      <c r="C593" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D593" s="1">
+        <v>20233256</v>
+      </c>
+      <c r="E593" s="1" t="s">
+        <v>1309</v>
+      </c>
+      <c r="F593" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G593" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H593" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I593" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J593" s="5">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="K593" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L593" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N593" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="594" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A594" s="2">
+        <v>45190.627843726848</v>
+      </c>
+      <c r="B594" s="1" t="s">
+        <v>1310</v>
+      </c>
+      <c r="C594" s="1" t="s">
+        <v>864</v>
+      </c>
+      <c r="D594" s="1">
+        <v>20221043</v>
+      </c>
+      <c r="E594" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="F594" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G594" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H594" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I594" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J594" s="5">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="K594" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L594" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N594" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="595" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A595" s="2">
+        <v>45190.632317638891</v>
+      </c>
+      <c r="B595" s="1" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C595" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D595" s="1">
+        <v>20232590</v>
+      </c>
+      <c r="E595" s="1" t="s">
+        <v>1313</v>
+      </c>
+      <c r="F595" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G595" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H595" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I595" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J595" s="5">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="K595" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L595" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M595" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="596" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A596" s="2">
+        <v>45190.692576458328</v>
+      </c>
+      <c r="B596" s="1" t="s">
+        <v>1314</v>
+      </c>
+      <c r="C596" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D596" s="1">
+        <v>20232537</v>
+      </c>
+      <c r="E596" s="1" t="s">
+        <v>1315</v>
+      </c>
+      <c r="F596" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G596" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H596" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I596" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J596" s="5">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="K596" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L596" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M596" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="597" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A597" s="2">
+        <v>45190.70098991898</v>
+      </c>
+      <c r="B597" s="1" t="s">
+        <v>1316</v>
+      </c>
+      <c r="C597" s="1" t="s">
+        <v>1317</v>
+      </c>
+      <c r="D597" s="1">
+        <v>20181205</v>
+      </c>
+      <c r="E597" s="1" t="s">
+        <v>1318</v>
+      </c>
+      <c r="F597" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G597" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H597" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I597" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J597" s="5">
+        <v>0.151</v>
+      </c>
+      <c r="K597" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L597" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M597" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="598" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A598" s="2">
+        <v>45190.750975717594</v>
+      </c>
+      <c r="B598" s="1" t="s">
+        <v>1319</v>
+      </c>
+      <c r="C598" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="D598" s="1">
+        <v>20215154</v>
+      </c>
+      <c r="E598" s="1" t="s">
+        <v>1320</v>
+      </c>
+      <c r="F598" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G598" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H598" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I598" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J598" s="5">
+        <v>0.151</v>
+      </c>
+      <c r="K598" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L598" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M598" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="599" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A599" s="2">
+        <v>45190.782722581018</v>
+      </c>
+      <c r="B599" s="1" t="s">
+        <v>1321</v>
+      </c>
+      <c r="C599" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D599" s="1">
+        <v>20226256</v>
+      </c>
+      <c r="E599" s="1" t="s">
+        <v>1322</v>
+      </c>
+      <c r="F599" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G599" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="H599" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I599" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J599" s="5">
+        <v>0.374</v>
+      </c>
+      <c r="K599" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L599" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M599" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="600" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A600" s="2">
+        <v>45190.789928113431</v>
+      </c>
+      <c r="B600" s="1" t="s">
+        <v>1323</v>
+      </c>
+      <c r="C600" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D600" s="1">
+        <v>20201634</v>
+      </c>
+      <c r="E600" s="1" t="s">
+        <v>1324</v>
+      </c>
+      <c r="F600" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G600" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H600" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I600" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J600" s="5">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="K600" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L600" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M600" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N334">
     <sortCondition ref="A1:A334"/>

</xml_diff>